<commit_message>
add link & update readme
</commit_message>
<xml_diff>
--- a/tools/cra/cra-proposal-annexes.xlsx
+++ b/tools/cra/cra-proposal-annexes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/cra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3024558A-1A6B-9F45-8CF0-C9E0FC69587B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE111A0-65B8-AA42-8CE8-7B5044D2E302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{4C543A3B-AB64-D642-BEBD-91CF67EC17E2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{4C543A3B-AB64-D642-BEBD-91CF67EC17E2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="362">
   <si>
     <t>assessable</t>
   </si>
@@ -1139,19 +1139,16 @@
   <si>
     <t>reference_control_base_urn</t>
   </si>
+  <si>
+    <t>ANNEXES to the PROPOSAL FOR A REGULATION OF THE EUROPEAN PARLIAMENT AND OF THE COUNCIL on horizontal cybersecurity requirements for products with digital elements and amending Regulation (EU) 2019/1020
+https://eur-lex.europa.eu/legal-content/EN/TXT/?uri=celex:52022PC0454</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1205,42 +1202,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1558,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBFB151-18DB-C34B-8ABC-829C94FCAAA9}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="275" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="275" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1608,12 +1602,12 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>340</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1704,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631939B4-A799-E14F-A776-21A901102AE8}">
   <dimension ref="A1:E212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="144" workbookViewId="0">
-      <selection activeCell="B209" sqref="B209"/>
+    <sheetView topLeftCell="B187" zoomScale="144" workbookViewId="0">
+      <selection activeCell="C210" sqref="C210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4628,7 +4622,7 @@
     </row>
     <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="6"/>
-      <c r="B209" s="13">
+      <c r="B209" s="6">
         <v>3</v>
       </c>
       <c r="C209" s="7" t="s">

</xml_diff>